<commit_message>
update to problem 20
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hoang Thang\Coding-Practice-LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Note\Coding-Practice-LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="89">
   <si>
     <t>#</t>
   </si>
@@ -122,9 +122,6 @@
     <t>https://leetcode.com/problems/longest-palindromic-substring/</t>
   </si>
   <si>
-    <t>O(log(min(m,n))</t>
-  </si>
-  <si>
     <t>O(n^2)</t>
   </si>
   <si>
@@ -140,13 +137,160 @@
     <t>Recursion</t>
   </si>
   <si>
-    <t>ad-hoc</t>
-  </si>
-  <si>
     <t>676ms(13.62%)</t>
   </si>
   <si>
     <t>32ms(77.49%)</t>
+  </si>
+  <si>
+    <t>manacher's algorithm</t>
+  </si>
+  <si>
+    <t>O(log(min(m,n)))</t>
+  </si>
+  <si>
+    <t>12ms(93.43%)</t>
+  </si>
+  <si>
+    <t>ZigZag Conversion</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/zigzag-conversion/</t>
+  </si>
+  <si>
+    <t>O(n*m)</t>
+  </si>
+  <si>
+    <t>n = s.length(), m = numRows</t>
+  </si>
+  <si>
+    <t>32ms(28.41%)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-integer/</t>
+  </si>
+  <si>
+    <t>Reverse Integer</t>
+  </si>
+  <si>
+    <t>O(log10(n) + 1)</t>
+  </si>
+  <si>
+    <t>String to Integer (atoi)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/string-to-integer-atoi/</t>
+  </si>
+  <si>
+    <t>Palindrome Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-number/</t>
+  </si>
+  <si>
+    <t>4ms(94.92%)</t>
+  </si>
+  <si>
+    <t>Regular Expression Matching</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/regular-expression-matching/</t>
+  </si>
+  <si>
+    <t>4ms(90.10%)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/container-with-most-water/</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>16ms(99.39%)</t>
+  </si>
+  <si>
+    <t>Integer to Roman</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/integer-to-roman/</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>12ms(47.31%)</t>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+  </si>
+  <si>
+    <t>Longest Common Prefix</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-common-prefix/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/roman-to-integer/</t>
+  </si>
+  <si>
+    <t>28 ms(28.02%)</t>
+  </si>
+  <si>
+    <t>4ms(93.05%)</t>
+  </si>
+  <si>
+    <t>72ms(92.48%)</t>
+  </si>
+  <si>
+    <t>3Sum Closest</t>
+  </si>
+  <si>
+    <t>Letter Combinations of a Phone Number</t>
+  </si>
+  <si>
+    <t>4Sum</t>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum-closest/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/letter-combinations-of-a-phone-number/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/4sum/</t>
+  </si>
+  <si>
+    <t>O(n^3)</t>
+  </si>
+  <si>
+    <t>4ms(99.95%)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-nth-node-from-end-of-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-parentheses/</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Ad-hoc</t>
   </si>
 </sst>
 </file>
@@ -219,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -268,12 +412,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -288,86 +452,431 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="57">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -707,386 +1216,742 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G8" sqref="G8"/>
+      <selection pane="topRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="75.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="75.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.140625" style="6" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="6"/>
-    <col min="20" max="20" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="6"/>
+    <col min="9" max="9" width="3.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.109375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-    </row>
-    <row r="2" spans="1:35" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="28" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+    </row>
+    <row r="2" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="Q2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="25"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="R2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" s="16"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="G3" s="7"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="G4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="G5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A6" s="27">
         <v>4</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="28" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="22"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
+        <v>5</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
-        <v>5</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="23"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="F11" s="15"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="6"/>
+      <c r="F10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="5"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>8</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>10</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>11</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>12</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>13</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>14</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>15</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P20" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>16</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>17</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>18</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="P23" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>19</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>20</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="S25" s="18" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H1:T1"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="D8:D10"/>
-    <mergeCell ref="H1:R1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A6:A7"/>
@@ -1100,40 +1965,205 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="56" priority="52" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1141,8 +2171,11 @@
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D5" r:id="rId2"/>
     <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D20" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add problem 60 -> 64
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
   <si>
     <t>#</t>
   </si>
@@ -56,9 +56,6 @@
     <t xml:space="preserve">Difficulty </t>
   </si>
   <si>
-    <t>Complexity</t>
-  </si>
-  <si>
     <t>O(n)</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>Greedy</t>
   </si>
   <si>
-    <t>Binary Search</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>BFS</t>
   </si>
   <si>
-    <t>Two Pointers</t>
-  </si>
-  <si>
     <t>Recursion</t>
   </si>
   <si>
@@ -291,6 +282,80 @@
   </si>
   <si>
     <t>Ad-hoc</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Data Structure</t>
+  </si>
+  <si>
+    <t>Two pointers</t>
+  </si>
+  <si>
+    <t>Divide and Conquer</t>
+  </si>
+  <si>
+    <t>Unique Paths II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths-ii/</t>
+  </si>
+  <si>
+    <t>O(m*n)</t>
+  </si>
+  <si>
+    <t>path[i][0] = (obstacleGrid[i][0] == 1) ? 0 : path[i-1][0] ( i: 0 -&gt; m)
+path[0][i] = (obstacleGrid[0][i] == 1) ? 0 : path[0][i-1] ( i: 0 -&gt; n)
+path[i][j] = (obstacleGrid[i][j] == 1) ? 0 : path[i-1][j] + path[i][j-1]</t>
+  </si>
+  <si>
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/</t>
+  </si>
+  <si>
+    <t>path[i][0] = 1 ( i: 0 -&gt; m); path[0][i] = 1 ( i: 0 -&gt; n)
+path[i][j] = path[i-1][j] + path[i][j-1]</t>
+  </si>
+  <si>
+    <t>Rotate List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-list/</t>
+  </si>
+  <si>
+    <t>Permutation Sequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutation-sequence/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pay attention to the total of permutation with n length is the factorial of n (n!). </t>
+  </si>
+  <si>
+    <t>Minimum Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-path-sum/</t>
+  </si>
+  <si>
+    <t>min_length[i][0] = min_length[i-1][0] + grid[i][0] ( i: 0 -&gt; m)
+min_length[0][i] = min_length[0][i-1] + grid[0][i] ( i: 0 -&gt; n)
+min_length[i][j] = std::min(min_length[i-1][j], min_length[i][j-1]) + grid[i][j]</t>
+  </si>
+  <si>
+    <t>8ms(98.62%)</t>
   </si>
 </sst>
 </file>
@@ -363,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -403,19 +468,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -440,9 +492,6 @@
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -490,36 +539,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -529,18 +575,108 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="69">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1216,744 +1352,953 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI25"/>
+  <dimension ref="A1:AO69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="75.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.109375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" style="18" customWidth="1"/>
+    <col min="12" max="12" width="6.77734375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="3" style="18" customWidth="1"/>
+    <col min="14" max="14" width="3.88671875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" style="18" customWidth="1"/>
+    <col min="16" max="24" width="15.77734375" style="7" customWidth="1"/>
+    <col min="25" max="26" width="15.77734375" style="3" customWidth="1"/>
+    <col min="27" max="27" width="13.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="74" style="2" customWidth="1"/>
+    <col min="42" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:41" s="18" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="X2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
+      <c r="AO2" s="29"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="H3" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="AA3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB3" s="6"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" s="3"/>
+      <c r="Z4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB4" s="6"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="3"/>
+      <c r="Z5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB5" s="6"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>4</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB6" s="6"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>5</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB8" s="6"/>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="20"/>
+      <c r="F9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB9" s="6"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="F10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="Z11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB11" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB12" s="6"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>8</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="Z13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA13" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA14" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>10</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="Z16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA16" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>12</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA17" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>13</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA18" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
         <v>14</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="B19" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA19" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>15</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA20" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>16</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA21" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>17</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA22" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>18</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA23" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>19</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA24" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>20</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA25" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
         <v>22</v>
       </c>
-      <c r="H1" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-    </row>
-    <row r="2" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="16" t="s">
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
         <v>34</v>
       </c>
-      <c r="P2" s="17" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
         <v>35</v>
       </c>
-      <c r="Q2" s="16" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
         <v>36</v>
       </c>
-      <c r="R2" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="T2" s="16"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="13" t="s">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A65" s="5">
+        <v>60</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="R65" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA65" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB65" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A66" s="5">
+        <v>61</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D66" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA66" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13" t="s">
+    </row>
+    <row r="67" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
+        <v>62</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>4</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="D67" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q67" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA67" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB67" s="32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5">
+        <v>63</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="D68" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q68" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA68" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB68" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
+        <v>64</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D69" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
-        <v>7</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="5"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>8</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
-        <v>9</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>10</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
-        <v>11</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>12</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
-        <v>13</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>14</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
-        <v>15</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="P20" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
-        <v>16</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="P21" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
-        <v>17</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q22" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
-        <v>18</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="P23" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
-        <v>19</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
-        <v>20</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="S25" s="18" t="s">
-        <v>33</v>
+      <c r="Q69" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA69" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB69" s="32" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H1:T1"/>
+    <mergeCell ref="E1:O1"/>
+    <mergeCell ref="P1:Z1"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -1961,209 +2306,263 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="56" priority="52" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C65)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C69)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C69)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",C69)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C65:C69">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add problem 66->70, 72, 82
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hoang Thang\Coding-Practice-LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Note\Coding-Practice-LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
   <si>
     <t>#</t>
   </si>
@@ -314,60 +314,112 @@
     <t>O(m*n)</t>
   </si>
   <si>
-    <t>path[i][0] = (obstacleGrid[i][0] == 1) ? 0 : path[i-1][0] ( i: 0 -&gt; m)
-path[0][i] = (obstacleGrid[0][i] == 1) ? 0 : path[0][i-1] ( i: 0 -&gt; n)
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/</t>
+  </si>
+  <si>
+    <t>Rotate List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-list/</t>
+  </si>
+  <si>
+    <t>Permutation Sequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutation-sequence/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pay attention to the total of permutation with n length is the factorial of n (n!). </t>
+  </si>
+  <si>
+    <t>Minimum Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-path-sum/</t>
+  </si>
+  <si>
+    <t>8ms(98.62%)</t>
+  </si>
+  <si>
+    <t>Valid Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-number/</t>
+  </si>
+  <si>
+    <t>Plus One</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/plus-one/</t>
+  </si>
+  <si>
+    <t>Add Binary</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-binary/</t>
+  </si>
+  <si>
+    <t>Sqrt(x)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sqrtx/</t>
+  </si>
+  <si>
+    <t>Edit Distance</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/edit-distance/</t>
+  </si>
+  <si>
+    <t>f[i][j]: minimum number of operations required to convert substring 0-&gt;i of word1 to substring 0-&gt;j of word2
+f[i][0] = i ( i: 0 -&gt; n ); f[0][i] = i ( i: 0 -&gt; m ); 
+f[i][j] = (word1[i - 1] == word2[j - 1]) ? f[i - 1][j - 1] : std::min(f[i - 1][j], std::min(f[i][j - 1], f[i - 1][j - 1])) + 1</t>
+  </si>
+  <si>
+    <t>path[i][j]: the number of unique paths from 0,0 to i,j
+path[i][0] = 1 ( i: 0 -&gt; m); path[0][i] = 1 ( i: 0 -&gt; n)
+path[i][j] = path[i-1][j] + path[i][j-1]</t>
+  </si>
+  <si>
+    <t>min_length[i][j]: the minimum sum from 0,0 to i,j 
+min_length[i][0] = min_length[i-1][0] + grid[i][0] ( i: 0 -&gt; m) ; min_length[0][i] = min_length[0][i-1] + grid[0][i] ( i: 0 -&gt; n)
+min_length[i][j] = std::min(min_length[i-1][j], min_length[i][j-1]) + grid[i][j]</t>
+  </si>
+  <si>
+    <t>path[i][j]: the number of unique paths from 0,0 to i,j
+path[i][0] = (obstacleGrid[i][0] == 1) ? 0 : path[i-1][0] ( i: 0 -&gt; m) ; path[0][i] = (obstacleGrid[0][i] == 1) ? 0 : path[0][i-1] ( i: 0 -&gt; n)
 path[i][j] = (obstacleGrid[i][j] == 1) ? 0 : path[i-1][j] + path[i][j-1]</t>
   </si>
   <si>
-    <t>Unique Paths</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/unique-paths/</t>
-  </si>
-  <si>
-    <t>path[i][0] = 1 ( i: 0 -&gt; m); path[0][i] = 1 ( i: 0 -&gt; n)
-path[i][j] = path[i-1][j] + path[i][j-1]</t>
-  </si>
-  <si>
-    <t>Rotate List</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/rotate-list/</t>
-  </si>
-  <si>
-    <t>Permutation Sequence</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/permutation-sequence/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pay attention to the total of permutation with n length is the factorial of n (n!). </t>
-  </si>
-  <si>
-    <t>Minimum Path Sum</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/minimum-path-sum/</t>
-  </si>
-  <si>
-    <t>min_length[i][0] = min_length[i-1][0] + grid[i][0] ( i: 0 -&gt; m)
-min_length[0][i] = min_length[0][i-1] + grid[0][i] ( i: 0 -&gt; n)
-min_length[i][j] = std::min(min_length[i-1][j], min_length[i][j-1]) + grid[i][j]</t>
-  </si>
-  <si>
-    <t>8ms(98.62%)</t>
-  </si>
-  <si>
-    <t>Valid Number</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/valid-number/</t>
-  </si>
-  <si>
-    <t>Plus One</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/plus-one/</t>
+    <t>Remove Duplicates from Sorted List II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/</t>
+  </si>
+  <si>
+    <t>O(max(n,m))</t>
+  </si>
+  <si>
+    <t>O(log(n))</t>
+  </si>
+  <si>
+    <t>Text Justification</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/text-justification/</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t>f[i]: the number of ways to climb stair i
+f[1] = 1; f[2] = 2; f[i] = f[i-1] + f[i-2];</t>
   </si>
 </sst>
 </file>
@@ -501,7 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -566,6 +618,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,15 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -607,7 +665,112 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="90">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1409,13 +1572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO71"/>
+  <dimension ref="A1:AO77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="W63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA71" sqref="AA71"/>
+      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1437,61 +1600,62 @@
     <col min="16" max="24" width="15.6640625" style="7" customWidth="1"/>
     <col min="25" max="26" width="15.6640625" style="3" customWidth="1"/>
     <col min="27" max="27" width="13.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="74" style="2" customWidth="1"/>
+    <col min="28" max="28" width="107.6640625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="93.88671875" customWidth="1"/>
     <col min="42" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="18" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="32" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="22" t="s">
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AB1" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="15" t="s">
         <v>86</v>
       </c>
@@ -1546,8 +1710,8 @@
         <v>92</v>
       </c>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="25"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="30"/>
       <c r="AC2" s="20"/>
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
@@ -1638,16 +1802,16 @@
       <c r="AB5" s="6"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A6" s="26">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="31" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1662,10 +1826,10 @@
       <c r="AB6" s="6"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1674,16 +1838,16 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A8" s="26">
+      <c r="A8" s="24">
         <v>5</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="25" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="18" t="s">
@@ -1698,10 +1862,10 @@
       <c r="AB8" s="6"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="27"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="25"/>
       <c r="F9" s="18" t="s">
         <v>31</v>
       </c>
@@ -1714,10 +1878,10 @@
       <c r="AB9" s="6"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="25"/>
       <c r="F10" s="18" t="s">
         <v>31</v>
       </c>
@@ -2226,13 +2390,13 @@
         <v>60</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R65" s="7" t="s">
         <v>30</v>
@@ -2241,7 +2405,7 @@
         <v>24</v>
       </c>
       <c r="AB65" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.3">
@@ -2249,13 +2413,13 @@
         <v>61</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G66" s="18" t="s">
         <v>31</v>
@@ -2267,18 +2431,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>62</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>31</v>
@@ -2290,7 +2454,7 @@
         <v>24</v>
       </c>
       <c r="AB67" s="21" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
@@ -2316,7 +2480,7 @@
         <v>24</v>
       </c>
       <c r="AB68" s="21" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
@@ -2324,13 +2488,13 @@
         <v>64</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>31</v>
@@ -2339,10 +2503,10 @@
         <v>95</v>
       </c>
       <c r="AA69" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AB69" s="21" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.3">
@@ -2350,16 +2514,19 @@
         <v>65</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>31</v>
+      </c>
+      <c r="Z70" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="AA70" s="11" t="s">
         <v>24</v>
@@ -2370,25 +2537,186 @@
         <v>66</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="Z71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA71" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A72" s="5">
+        <v>67</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F72" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z72" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA72" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A73" s="22">
+        <v>68</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="22"/>
+      <c r="L73" s="22"/>
+      <c r="M73" s="22"/>
+      <c r="N73" s="22"/>
+      <c r="O73" s="22"/>
+      <c r="Z73" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA73" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
+        <v>69</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z74" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA74" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="22">
+        <v>70</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="22"/>
+      <c r="L75" s="22"/>
+      <c r="M75" s="22"/>
+      <c r="N75" s="22"/>
+      <c r="O75" s="22"/>
+      <c r="Q75" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA75" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB75" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="22">
+        <v>72</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F76" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q76" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA76" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB76" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A77" s="5">
+        <v>82</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G77" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z77" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA77" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -2400,284 +2728,344 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:O1"/>
     <mergeCell ref="P1:Z1"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="89" priority="88" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C71)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C71)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C72">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C72)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C72)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74:C75">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C74)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C74)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C74)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C76)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C76)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C76)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C77)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C77)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C77)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",C73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C65:C71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C65:C77">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add problem 50->59, 71->76, 88,91,98
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="175">
   <si>
     <t>#</t>
   </si>
@@ -420,6 +420,145 @@
   <si>
     <t>f[i]: the number of ways to climb stair i
 f[1] = 1; f[2] = 2; f[i] = f[i-1] + f[i-2];</t>
+  </si>
+  <si>
+    <t>Pow(x, n)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/powx-n/</t>
+  </si>
+  <si>
+    <t>x^n = ( n % 2 == 0 ) ? x^(n/2) * x^(n/2) : x^(n/2) * x^(n/2) * x</t>
+  </si>
+  <si>
+    <t>N-Queens</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/n-queens/</t>
+  </si>
+  <si>
+    <t>8ms(74.30%)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/n-queens-ii/</t>
+  </si>
+  <si>
+    <t>N-Queens II</t>
+  </si>
+  <si>
+    <t>4ms(85.83%)</t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/</t>
+  </si>
+  <si>
+    <t>sum[i]: the sum of elements from 0 -&gt; i ; min[i]: the minimum elements from 0 -&gt; i 
+result = max( sum[i] - min[i] )</t>
+  </si>
+  <si>
+    <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/spiral-matrix/</t>
+  </si>
+  <si>
+    <t>Jump Game</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/jump-game/</t>
+  </si>
+  <si>
+    <t>4ms(99.73%)</t>
+  </si>
+  <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-intervals/</t>
+  </si>
+  <si>
+    <t>28ms(88.07%)</t>
+  </si>
+  <si>
+    <t>Insert Interval</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-interval/</t>
+  </si>
+  <si>
+    <t>24ms(78.46%)</t>
+  </si>
+  <si>
+    <t>Length of Last Word</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/length-of-last-word/</t>
+  </si>
+  <si>
+    <t>Spiral Matrix II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/spiral-matrix-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-sorted-array/</t>
+  </si>
+  <si>
+    <t>O(n+m)</t>
+  </si>
+  <si>
+    <t>Decode Ways</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/decode-ways/</t>
+  </si>
+  <si>
+    <t>BST</t>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/validate-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>8ms(98.16%)</t>
+  </si>
+  <si>
+    <t>Simplify Path</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/simplify-path/</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/set-matrix-zeroes/</t>
+  </si>
+  <si>
+    <t>8ms(99.66%)</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-a-2d-matrix/</t>
+  </si>
+  <si>
+    <t>O(log(m*n))</t>
+  </si>
+  <si>
+    <t>Sort Colors</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-colors/</t>
   </si>
 </sst>
 </file>
@@ -553,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -630,20 +769,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -660,12 +799,333 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="135">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1572,13 +2032,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO77"/>
+  <dimension ref="A1:AO84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
+      <selection pane="bottomRight" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1592,7 +2052,7 @@
     <col min="7" max="7" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.44140625" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="5.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" style="18" customWidth="1"/>
+    <col min="11" max="11" width="4" style="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.6640625" style="18" customWidth="1"/>
     <col min="13" max="13" width="3" style="18" customWidth="1"/>
     <col min="14" max="14" width="3.88671875" style="18" customWidth="1"/>
@@ -1618,19 +2078,19 @@
       <c r="D1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
       <c r="P1" s="34" t="s">
         <v>14</v>
       </c>
@@ -1644,10 +2104,10 @@
       <c r="X1" s="35"/>
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="29" t="s">
+      <c r="AB1" s="26" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1674,7 +2134,9 @@
       <c r="J2" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="16"/>
+      <c r="K2" s="16" t="s">
+        <v>161</v>
+      </c>
       <c r="L2" s="15"/>
       <c r="M2" s="16"/>
       <c r="N2" s="15"/>
@@ -1710,8 +2172,8 @@
         <v>92</v>
       </c>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="30"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="27"/>
       <c r="AC2" s="20"/>
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
@@ -1802,13 +2264,13 @@
       <c r="AB5" s="6"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A6" s="24">
+      <c r="A6" s="28">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="31" t="s">
@@ -1826,9 +2288,9 @@
       <c r="AB6" s="6"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="31"/>
       <c r="E7" s="1" t="s">
         <v>31</v>
@@ -1838,16 +2300,16 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
+      <c r="A8" s="28">
         <v>5</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="29" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="18" t="s">
@@ -1862,10 +2324,10 @@
       <c r="AB8" s="6"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="25"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="29"/>
       <c r="F9" s="18" t="s">
         <v>31</v>
       </c>
@@ -1878,10 +2340,10 @@
       <c r="AB9" s="6"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="29"/>
       <c r="F10" s="18" t="s">
         <v>31</v>
       </c>
@@ -2305,84 +2767,261 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y55" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA55" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB55" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>51</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="X56" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA56" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>52</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="X57" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA57" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB58" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z59" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA59" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V60" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA60" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA61" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA62" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA63" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>59</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z64" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA64" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.3">
@@ -2666,57 +3305,260 @@
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="22">
-        <v>72</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>114</v>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A76" s="24">
+        <v>71</v>
+      </c>
+      <c r="B76" s="25" t="s">
+        <v>165</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F76" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F76" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="Q76" s="7" t="s">
-        <v>95</v>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="24"/>
+      <c r="L76" s="24"/>
+      <c r="M76" s="24"/>
+      <c r="N76" s="24"/>
+      <c r="O76" s="24"/>
+      <c r="Z76" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="AA76" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AB76" s="21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A77" s="5">
-        <v>82</v>
-      </c>
-      <c r="B77" s="23" t="s">
-        <v>120</v>
+      <c r="AB76" s="21"/>
+    </row>
+    <row r="77" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="22">
+        <v>72</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G77" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F77" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="Z77" s="3" t="s">
-        <v>10</v>
+      <c r="Q77" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="AA77" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="AB77" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A78" s="24">
+        <v>73</v>
+      </c>
+      <c r="B78" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="24"/>
+      <c r="L78" s="24"/>
+      <c r="M78" s="24"/>
+      <c r="N78" s="24"/>
+      <c r="O78" s="24"/>
+      <c r="AA78" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB78" s="21"/>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A79" s="24">
+        <v>74</v>
+      </c>
+      <c r="B79" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="K79" s="24"/>
+      <c r="L79" s="24"/>
+      <c r="M79" s="24"/>
+      <c r="N79" s="24"/>
+      <c r="O79" s="24"/>
+      <c r="Z79" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA79" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB79" s="21"/>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A80" s="24">
+        <v>75</v>
+      </c>
+      <c r="B80" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="24"/>
+      <c r="N80" s="24"/>
+      <c r="O80" s="24"/>
+      <c r="Z80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA80" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB80" s="21"/>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
+        <v>82</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G81" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z81" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA81" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
+        <v>88</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W82" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA82" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
+        <v>91</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q83" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA83" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A84" s="5">
+        <v>98</v>
+      </c>
+      <c r="B84" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="K84" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA84" s="10" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -2728,344 +3570,504 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:O1"/>
     <mergeCell ref="P1:Z1"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
+    <cfRule type="containsText" dxfId="134" priority="133" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="134" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="135" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C6">
+    <cfRule type="containsText" dxfId="131" priority="130" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="128" priority="127" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="125" priority="124" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="122" priority="121" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsText" dxfId="119" priority="118" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="containsText" dxfId="116" priority="115" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="113" priority="112" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="containsText" dxfId="110" priority="109" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="containsText" dxfId="107" priority="106" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="104" priority="103" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="101" priority="100" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="98" priority="97" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="containsText" dxfId="95" priority="94" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="containsText" dxfId="92" priority="91" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="93" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
     <cfRule type="containsText" dxfId="89" priority="88" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C6">
+      <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
     <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+      <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
     <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
+      <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
     <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C68)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C68)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+      <formula>NOT(ISERROR(SEARCH("Easy",C68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
     <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C67)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C67)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+      <formula>NOT(ISERROR(SEARCH("Easy",C67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
     <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C66)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C66)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+      <formula>NOT(ISERROR(SEARCH("Easy",C66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
     <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+      <formula>NOT(ISERROR(SEARCH("Easy",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69">
     <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C69)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C69)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+      <formula>NOT(ISERROR(SEARCH("Easy",C69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70">
     <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C70)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C70)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+      <formula>NOT(ISERROR(SEARCH("Easy",C70)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71">
     <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+      <formula>NOT(ISERROR(SEARCH("Easy",C71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C72">
     <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C72)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C72)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+      <formula>NOT(ISERROR(SEARCH("Easy",C72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74:C75">
     <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C74)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C74)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+      <formula>NOT(ISERROR(SEARCH("Easy",C74)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
     <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C77)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C77)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+      <formula>NOT(ISERROR(SEARCH("Easy",C77)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C81">
     <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C81)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C81)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+      <formula>NOT(ISERROR(SEARCH("Easy",C81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73">
     <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
+      <formula>NOT(ISERROR(SEARCH("Easy",C73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
     <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
+      <formula>NOT(ISERROR(SEARCH("Easy",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
     <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
+      <formula>NOT(ISERROR(SEARCH("Easy",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
     <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C57)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C57)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
+      <formula>NOT(ISERROR(SEARCH("Easy",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C68)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C68)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C68)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
+      <formula>NOT(ISERROR(SEARCH("Easy",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
     <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C67)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C67)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
+      <formula>NOT(ISERROR(SEARCH("Easy",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
     <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C60)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C60)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C66)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
+      <formula>NOT(ISERROR(SEARCH("Easy",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C65)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C65)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C69">
+      <formula>NOT(ISERROR(SEARCH("Easy",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
     <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C69)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
+      <formula>NOT(ISERROR(SEARCH("Easy",C62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
     <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C70)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C63)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C70)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C63)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C70)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
+      <formula>NOT(ISERROR(SEARCH("Easy",C63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
     <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C71)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C72">
+      <formula>NOT(ISERROR(SEARCH("Easy",C64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82">
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C72)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C82)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C72)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C82)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C74:C75">
+      <formula>NOT(ISERROR(SEARCH("Easy",C82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C83">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C74)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C83)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C74)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C83)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C74)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",C83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C84)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C84)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C76)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C77)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C77)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C77)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
+  <conditionalFormatting sqref="C78:C80">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C73)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C78)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C73)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C78)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C73)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",C78)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C65:C77">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C55:C84">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add problem 45->49, 77,78
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="196">
   <si>
     <t>#</t>
   </si>
@@ -559,6 +559,69 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/sort-colors/</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-window-substring/</t>
+  </si>
+  <si>
+    <t>16ms(70.06%)</t>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/group-anagrams/</t>
+  </si>
+  <si>
+    <t>36ms(93.53%)</t>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-image/</t>
+  </si>
+  <si>
+    <t>Permutations II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutations-ii/</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Permutations</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutations/</t>
+  </si>
+  <si>
+    <t>Jump Game II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/jump-game-ii/</t>
+  </si>
+  <si>
+    <t>8ms(99.40%)</t>
+  </si>
+  <si>
+    <t>Combinations</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combinations/</t>
+  </si>
+  <si>
+    <t>12ms(93.57%)</t>
+  </si>
+  <si>
+    <t>Subsets</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets/</t>
   </si>
 </sst>
 </file>
@@ -692,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -769,11 +832,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -783,6 +846,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -799,18 +874,180 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
+  <dxfs count="159">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2032,13 +2269,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO84"/>
+  <dimension ref="A1:AO87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="W42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D76" sqref="D76"/>
+      <selection pane="bottomRight" activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2066,56 +2303,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="18" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="34" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="36" t="s">
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AB1" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="15" t="s">
         <v>86</v>
       </c>
@@ -2137,7 +2374,9 @@
       <c r="K2" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="L2" s="15"/>
+      <c r="L2" s="15" t="s">
+        <v>185</v>
+      </c>
       <c r="M2" s="16"/>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
@@ -2172,8 +2411,8 @@
         <v>92</v>
       </c>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="27"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="34"/>
       <c r="AC2" s="20"/>
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
@@ -2273,7 +2512,7 @@
       <c r="C6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="35" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -2291,7 +2530,7 @@
       <c r="A7" s="28"/>
       <c r="B7" s="29"/>
       <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
@@ -2776,25 +3015,118 @@
       <c r="A50" s="5">
         <v>45</v>
       </c>
+      <c r="B50" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L50" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="V50" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA50" s="10" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>46</v>
       </c>
+      <c r="B51" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L51" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA51" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>47</v>
       </c>
+      <c r="B52" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L52" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="X52" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA52" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>48</v>
       </c>
+      <c r="B53" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA53" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>49</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA54" s="10" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.3">
@@ -3463,102 +3795,197 @@
       </c>
       <c r="AB80" s="21"/>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A81" s="5">
-        <v>82</v>
-      </c>
-      <c r="B81" s="23" t="s">
-        <v>120</v>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A81" s="26">
+        <v>76</v>
+      </c>
+      <c r="B81" s="27" t="s">
+        <v>175</v>
       </c>
       <c r="C81" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F81" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I81" s="26"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="26"/>
+      <c r="L81" s="26"/>
+      <c r="M81" s="26"/>
+      <c r="N81" s="26"/>
+      <c r="O81" s="26"/>
+      <c r="W81" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA81" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB81" s="21"/>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A82" s="26">
+        <v>77</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C82" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G81" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z81" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA81" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A82" s="5">
-        <v>88</v>
-      </c>
-      <c r="B82" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>6</v>
-      </c>
       <c r="D82" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W82" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA82" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A83" s="5">
-        <v>91</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>158</v>
+        <v>192</v>
+      </c>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="26"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="26"/>
+      <c r="L82" s="26"/>
+      <c r="M82" s="26"/>
+      <c r="N82" s="26"/>
+      <c r="O82" s="26"/>
+      <c r="X82" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA82" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB82" s="21"/>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A83" s="26">
+        <v>78</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>194</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q83" s="7" t="s">
-        <v>10</v>
+        <v>195</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F83" s="26"/>
+      <c r="G83" s="26"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="26"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="26"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="26"/>
+      <c r="N83" s="26"/>
+      <c r="O83" s="26"/>
+      <c r="X83" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="AA83" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AB83" s="21"/>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
-        <v>98</v>
-      </c>
-      <c r="B84" s="25" t="s">
-        <v>162</v>
+        <v>82</v>
+      </c>
+      <c r="B84" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D84" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G84" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA84" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A85" s="5">
+        <v>88</v>
+      </c>
+      <c r="B85" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W85" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA85" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A86" s="5">
+        <v>91</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q86" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA86" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A87" s="5">
+        <v>98</v>
+      </c>
+      <c r="B87" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="K84" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA84" s="10" t="s">
+      <c r="K87" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA87" s="10" t="s">
         <v>164</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -3570,504 +3997,586 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:O1"/>
     <mergeCell ref="P1:Z1"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="134" priority="133" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="158" priority="154" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="134" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="157" priority="155" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="135" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="156" priority="156" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="containsText" dxfId="131" priority="130" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="155" priority="151" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="154" priority="152" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="153" priority="153" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="128" priority="127" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="152" priority="148" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="151" priority="149" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="150" priority="150" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="containsText" dxfId="125" priority="124" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="149" priority="145" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="148" priority="146" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="147" priority="147" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="122" priority="121" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="146" priority="142" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="145" priority="143" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="144" priority="144" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="containsText" dxfId="119" priority="118" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="143" priority="139" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="142" priority="140" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="141" priority="141" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="116" priority="115" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="140" priority="136" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="139" priority="137" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="138" priority="138" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="113" priority="112" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="137" priority="133" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="136" priority="134" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="135" priority="135" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="110" priority="109" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="134" priority="130" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="133" priority="131" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="132" priority="132" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="107" priority="106" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="131" priority="127" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="130" priority="128" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="129" priority="129" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="104" priority="103" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="128" priority="124" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="127" priority="125" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="126" priority="126" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="101" priority="100" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="125" priority="121" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="124" priority="122" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="123" priority="123" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="98" priority="97" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="122" priority="118" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="121" priority="119" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="120" priority="120" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" dxfId="95" priority="94" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="119" priority="115" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="118" priority="116" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="117" priority="117" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="containsText" dxfId="92" priority="91" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="116" priority="112" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="115" priority="113" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="93" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="114" priority="114" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="containsText" dxfId="89" priority="88" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="113" priority="109" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="112" priority="110" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="111" priority="111" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="110" priority="106" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="109" priority="107" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="108" priority="108" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="107" priority="103" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="106" priority="104" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="105" priority="105" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="104" priority="100" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="103" priority="101" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="102" priority="102" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="101" priority="97" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="100" priority="98" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="99" priority="99" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="98" priority="94" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="97" priority="95" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="96" priority="96" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="95" priority="91" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="94" priority="92" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="93" priority="93" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="92" priority="88" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="91" priority="89" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="90" priority="90" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="89" priority="85" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="88" priority="86" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="86" priority="82" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="85" priority="83" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C71)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="84" priority="84" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="83" priority="79" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C72)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="82" priority="80" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C72)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="81" priority="81" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74:C75">
-    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="80" priority="76" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="79" priority="77" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="78" priority="78" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="77" priority="73" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="76" priority="74" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="75" priority="75" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C77)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C84">
+    <cfRule type="containsText" dxfId="74" priority="70" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C84)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="71" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C84)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="72" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C84)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73">
+    <cfRule type="containsText" dxfId="71" priority="67" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C73)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C73)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="containsText" dxfId="68" priority="64" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="65" priority="61" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="62" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="containsText" dxfId="62" priority="58" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="containsText" dxfId="59" priority="55" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="56" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="56" priority="52" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C85">
+    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C85)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C85)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C85)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C86">
+    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C86)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C86)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C86)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87">
+    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C87)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C87)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C76)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C76)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C76)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C78:C80">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C81)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
-    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C73)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C73)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C73)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C55)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C56)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C57)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C58)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C59)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C60)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C62)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C63)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C64)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C83">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C82)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C83)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C83)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C83)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C84)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C84)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C84)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C76)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C78:C80">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C78)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C78)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C78)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C55:C84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C50:C87">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add problem first week of June
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Note\Coding-Practice-LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hoang Thang\Coding-Practice-LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="269">
   <si>
     <t>#</t>
   </si>
@@ -836,6 +836,60 @@
   </si>
   <si>
     <t>8ms(84.79%)</t>
+  </si>
+  <si>
+    <t>Maximum Performance of a Team</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-performance-of-a-team/</t>
+  </si>
+  <si>
+    <t>O(nlog(n))</t>
+  </si>
+  <si>
+    <t>48ms(100.0%)</t>
+  </si>
+  <si>
+    <t>Using sort to keep track of the engineers by their efficiency in decreasing order (O(nlogn)). Then with each engineer, to get maximum performance, let choose engineers who have higher efficiencies as well as high speeds (O(n)).</t>
+  </si>
+  <si>
+    <t>Open The Lock</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/open-the-lock/</t>
+  </si>
+  <si>
+    <t>24ms(98.17%)</t>
+  </si>
+  <si>
+    <t>Maximum Area of a Piece of Cake After Horizontal and Vertical Cuts</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-area-of-a-piece-of-cake-after-horizontal-and-vertical-cuts/</t>
+  </si>
+  <si>
+    <t>36ms(99.95%)</t>
+  </si>
+  <si>
+    <t>Max Area of Island</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/max-area-of-island/</t>
+  </si>
+  <si>
+    <t>12ms(97.17%)</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-consecutive-sequence/</t>
+  </si>
+  <si>
+    <t>124ms(34.22%)</t>
+  </si>
+  <si>
+    <t>Due to the time complexity is O(n) =&gt; we can't use sort. Besides, the limit of value is 10^9, so we maybe will use a hashmap instead of using an array to check value is exist.</t>
   </si>
 </sst>
 </file>
@@ -969,7 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1074,6 +1128,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1114,7 +1174,112 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="201">
+  <dxfs count="216">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2798,90 +2963,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO105"/>
+  <dimension ref="A1:AO110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E99" sqref="E99"/>
+      <selection pane="bottomRight" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="5.5546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" style="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.88671875" style="18" customWidth="1"/>
     <col min="15" max="15" width="4.33203125" style="18" customWidth="1"/>
-    <col min="16" max="24" width="15.6640625" style="7" customWidth="1"/>
-    <col min="25" max="26" width="15.6640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="107.6640625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="188.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="93.88671875" customWidth="1"/>
     <col min="42" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="18" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:41" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="45" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="38" t="s">
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="40" t="s">
+      <c r="AB1" s="42" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="15" t="s">
         <v>86</v>
       </c>
@@ -2942,8 +3117,8 @@
         <v>92</v>
       </c>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="43"/>
       <c r="AC2" s="20"/>
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
@@ -3034,16 +3209,16 @@
       <c r="AB5" s="6"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A6" s="35">
+      <c r="A6" s="37">
         <v>4</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="44" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -3058,10 +3233,10 @@
       <c r="AB6" s="6"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="42"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
@@ -3070,16 +3245,16 @@
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A8" s="35">
+      <c r="A8" s="37">
         <v>5</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="38" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="18" t="s">
@@ -3094,10 +3269,10 @@
       <c r="AB8" s="6"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="36"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="38"/>
       <c r="F9" s="18" t="s">
         <v>31</v>
       </c>
@@ -3110,10 +3285,10 @@
       <c r="AB9" s="6"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="36"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="38"/>
       <c r="F10" s="18" t="s">
         <v>31</v>
       </c>
@@ -4591,7 +4766,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="30">
         <v>84</v>
       </c>
@@ -4626,7 +4801,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A90" s="30">
         <v>85</v>
       </c>
@@ -5078,7 +5253,119 @@
         <v>250</v>
       </c>
     </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A106" s="5">
+        <v>128</v>
+      </c>
+      <c r="B106" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="H106" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA106" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="AB106" s="21" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A107" s="5">
+        <v>695</v>
+      </c>
+      <c r="B107" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA107" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A108" s="5">
+        <v>752</v>
+      </c>
+      <c r="B108" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="V108" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA108" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A109" s="5">
+        <v>1383</v>
+      </c>
+      <c r="B109" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="J109" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="T109" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA109" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB109" s="21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A110" s="5">
+        <v>1465</v>
+      </c>
+      <c r="B110" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="AA110" s="10" t="s">
+        <v>261</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A106:AO110">
+    <sortCondition ref="A106:A110"/>
+  </sortState>
   <mergeCells count="16">
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="A6:A7"/>
@@ -5098,744 +5385,799 @@
     <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
+    <cfRule type="containsText" dxfId="215" priority="214" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="214" priority="215" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="213" priority="216" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C6">
+    <cfRule type="containsText" dxfId="212" priority="211" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="211" priority="212" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="210" priority="213" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="209" priority="208" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="208" priority="209" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="207" priority="210" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="206" priority="205" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="205" priority="206" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="204" priority="207" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="203" priority="202" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="202" priority="203" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="201" priority="204" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
     <cfRule type="containsText" dxfId="200" priority="199" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="199" priority="200" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="198" priority="201" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C6">
+      <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
     <cfRule type="containsText" dxfId="197" priority="196" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="196" priority="197" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="195" priority="198" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+      <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
     <cfRule type="containsText" dxfId="194" priority="193" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="193" priority="194" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="192" priority="195" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
+      <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
     <cfRule type="containsText" dxfId="191" priority="190" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="190" priority="191" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="189" priority="192" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+      <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
     <cfRule type="containsText" dxfId="188" priority="187" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="187" priority="188" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="186" priority="189" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+      <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
     <cfRule type="containsText" dxfId="185" priority="184" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="184" priority="185" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="183" priority="186" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+      <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
     <cfRule type="containsText" dxfId="182" priority="181" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="181" priority="182" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="180" priority="183" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+      <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
     <cfRule type="containsText" dxfId="179" priority="178" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="178" priority="179" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="177" priority="180" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+      <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
     <cfRule type="containsText" dxfId="176" priority="175" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="175" priority="176" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="174" priority="177" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+      <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
     <cfRule type="containsText" dxfId="173" priority="172" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="172" priority="173" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="171" priority="174" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+      <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
     <cfRule type="containsText" dxfId="170" priority="169" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="169" priority="170" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="168" priority="171" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+      <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
     <cfRule type="containsText" dxfId="167" priority="166" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C19)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="166" priority="167" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C19)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="165" priority="168" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+      <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
     <cfRule type="containsText" dxfId="164" priority="163" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="163" priority="164" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="162" priority="165" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+      <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
     <cfRule type="containsText" dxfId="161" priority="160" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C68)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="160" priority="161" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C25)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C68)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="159" priority="162" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+      <formula>NOT(ISERROR(SEARCH("Easy",C68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
     <cfRule type="containsText" dxfId="158" priority="157" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C67)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="157" priority="158" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C67)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="156" priority="159" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
+      <formula>NOT(ISERROR(SEARCH("Easy",C67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
     <cfRule type="containsText" dxfId="155" priority="154" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C66)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="154" priority="155" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C66)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="153" priority="156" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
+      <formula>NOT(ISERROR(SEARCH("Easy",C66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
     <cfRule type="containsText" dxfId="152" priority="151" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="151" priority="152" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="150" priority="153" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
+      <formula>NOT(ISERROR(SEARCH("Easy",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69">
     <cfRule type="containsText" dxfId="149" priority="148" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C69)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="148" priority="149" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C24)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C69)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="147" priority="150" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
+      <formula>NOT(ISERROR(SEARCH("Easy",C69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70">
     <cfRule type="containsText" dxfId="146" priority="145" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C68)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C70)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="145" priority="146" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C68)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C70)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="144" priority="147" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C68)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
+      <formula>NOT(ISERROR(SEARCH("Easy",C70)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71">
     <cfRule type="containsText" dxfId="143" priority="142" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C67)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="142" priority="143" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C67)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="141" priority="144" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
+      <formula>NOT(ISERROR(SEARCH("Easy",C71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C72">
     <cfRule type="containsText" dxfId="140" priority="139" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C72)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="139" priority="140" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C72)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="138" priority="141" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C66)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
+      <formula>NOT(ISERROR(SEARCH("Easy",C72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74:C75">
     <cfRule type="containsText" dxfId="137" priority="136" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C65)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C74)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="136" priority="137" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C65)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C74)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="135" priority="138" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C69">
+      <formula>NOT(ISERROR(SEARCH("Easy",C74)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
     <cfRule type="containsText" dxfId="134" priority="133" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C77)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="133" priority="134" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C77)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="132" priority="135" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C69)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
+      <formula>NOT(ISERROR(SEARCH("Easy",C77)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87">
     <cfRule type="containsText" dxfId="131" priority="130" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C70)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C87)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C70)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C87)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C70)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
+      <formula>NOT(ISERROR(SEARCH("Easy",C87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73">
     <cfRule type="containsText" dxfId="128" priority="127" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C73)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C71)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C72">
+      <formula>NOT(ISERROR(SEARCH("Easy",C73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
     <cfRule type="containsText" dxfId="125" priority="124" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C72)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C72)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C74:C75">
+      <formula>NOT(ISERROR(SEARCH("Easy",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
     <cfRule type="containsText" dxfId="122" priority="121" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C74)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C74)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C56)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C74)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+      <formula>NOT(ISERROR(SEARCH("Easy",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
     <cfRule type="containsText" dxfId="119" priority="118" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C77)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C57)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C77)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C57)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C77)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C87">
+      <formula>NOT(ISERROR(SEARCH("Easy",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="116" priority="115" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C87)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C87)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C87)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
+      <formula>NOT(ISERROR(SEARCH("Easy",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
     <cfRule type="containsText" dxfId="113" priority="112" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C73)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C73)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C73)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
+      <formula>NOT(ISERROR(SEARCH("Easy",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
     <cfRule type="containsText" dxfId="110" priority="109" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C60)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C60)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("Easy",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="107" priority="106" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
+      <formula>NOT(ISERROR(SEARCH("Easy",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
     <cfRule type="containsText" dxfId="104" priority="103" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
+      <formula>NOT(ISERROR(SEARCH("Easy",C62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
     <cfRule type="containsText" dxfId="101" priority="100" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C63)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C63)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+      <formula>NOT(ISERROR(SEARCH("Easy",C63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
     <cfRule type="containsText" dxfId="98" priority="97" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C59)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C59)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("Easy",C64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C93">
     <cfRule type="containsText" dxfId="95" priority="94" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C60)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C93)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C60)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C93)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
+      <formula>NOT(ISERROR(SEARCH("Easy",C93)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C96:C98">
     <cfRule type="containsText" dxfId="92" priority="91" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C96)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C96)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="90" priority="93" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
+      <formula>NOT(ISERROR(SEARCH("Easy",C96)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C103">
     <cfRule type="containsText" dxfId="89" priority="88" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C103)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C103)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
+      <formula>NOT(ISERROR(SEARCH("Easy",C103)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76">
     <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C76)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C76)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
+      <formula>NOT(ISERROR(SEARCH("Easy",C76)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C78:C80">
     <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C64)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C78)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C64)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C78)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C93">
+      <formula>NOT(ISERROR(SEARCH("Easy",C78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C81">
     <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C93)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C81)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C93)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C81)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C93)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C96:C98">
+      <formula>NOT(ISERROR(SEARCH("Easy",C81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
     <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C96)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C96)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C96)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C103">
+      <formula>NOT(ISERROR(SEARCH("Easy",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
     <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C53)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C53)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C103)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
-    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C76)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C78:C80">
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C78)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C78)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C78)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C81">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
+      <formula>NOT(ISERROR(SEARCH("Easy",C53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="containsText" dxfId="71" priority="64" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="65" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="66" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C83">
     <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C82)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C82)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
+      <formula>NOT(ISERROR(SEARCH("Easy",C82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84">
     <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C84)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C84)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="56" priority="49" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C50)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="50" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C50)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="51" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C52)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="57" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C83">
+      <formula>NOT(ISERROR(SEARCH("Easy",C84)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C85">
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C85)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C85)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C85)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C86">
+    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C86)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C86)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C86)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88">
     <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C82)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C88)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C82)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C88)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+      <formula>NOT(ISERROR(SEARCH("Easy",C88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89:C90">
     <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C84)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C89)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C84)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C89)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C84)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+      <formula>NOT(ISERROR(SEARCH("Easy",C89)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
     <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C85)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C91)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C85)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C91)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C85)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+      <formula>NOT(ISERROR(SEARCH("Easy",C91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C92">
     <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C92)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C92)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C86">
+      <formula>NOT(ISERROR(SEARCH("Easy",C92)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C94">
     <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C86)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C86)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C86)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C88">
+      <formula>NOT(ISERROR(SEARCH("Easy",C94)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C95">
     <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C88)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C89:C90">
+      <formula>NOT(ISERROR(SEARCH("Easy",C95)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C99:C100">
     <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C89)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C99)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C89)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C99)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C89)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91">
+      <formula>NOT(ISERROR(SEARCH("Easy",C99)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C101">
     <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C91)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C101)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C91)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C101)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C91)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C92">
+      <formula>NOT(ISERROR(SEARCH("Easy",C101)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C102">
     <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C92)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C92)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C92)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C94">
+      <formula>NOT(ISERROR(SEARCH("Easy",C102)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C104">
     <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C94)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
+      <formula>NOT(ISERROR(SEARCH("Easy",C104)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C105">
     <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C95)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C105)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C95)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C105)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C95)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C99:C100">
+      <formula>NOT(ISERROR(SEARCH("Easy",C105)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C106">
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C99)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C106)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C99)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C106)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C99)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
+      <formula>NOT(ISERROR(SEARCH("Easy",C106)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C107">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C101)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C101)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C101)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
+      <formula>NOT(ISERROR(SEARCH("Easy",C107)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C108">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C108)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C108)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C102)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C104">
+      <formula>NOT(ISERROR(SEARCH("Easy",C108)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C109">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C104)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C104)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C104)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C105">
+      <formula>NOT(ISERROR(SEARCH("Easy",C109)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C110">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",C105)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",C110)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C105)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",C110)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",C105)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",C110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C38 C50:C105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C8 C11:C25 C38 C50:C110">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5876,8 +6218,13 @@
     <hyperlink ref="D66" r:id="rId34"/>
     <hyperlink ref="D104" r:id="rId35"/>
     <hyperlink ref="D105" r:id="rId36"/>
+    <hyperlink ref="D109" r:id="rId37"/>
+    <hyperlink ref="D108" r:id="rId38"/>
+    <hyperlink ref="D110" r:id="rId39"/>
+    <hyperlink ref="D107" r:id="rId40"/>
+    <hyperlink ref="D106" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>